<commit_message>
se ordeno los js, se conecta el html con los filtros del js, sin embargo aun no se imprime en html
</commit_message>
<xml_diff>
--- a/ProyectoFinal/Libro1.xlsx
+++ b/ProyectoFinal/Libro1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nessa\OneDrive\Escritorio\MisProyectos\Bootcamp\BootcampMakaia\ProyectoFinal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DBCEFAE0-F444-4C71-81CC-64C6AB21B50A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89823364-3682-4B50-9A08-0C6D9A1B85B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="350" yWindow="50" windowWidth="8480" windowHeight="10070" xr2:uid="{3761D6BA-73E2-48D3-BD59-D312106DBE04}"/>
+    <workbookView xWindow="-250" yWindow="490" windowWidth="10400" windowHeight="10070" xr2:uid="{3761D6BA-73E2-48D3-BD59-D312106DBE04}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="72">
   <si>
     <t>nombre</t>
   </si>
@@ -112,9 +112,6 @@
     <t>Luxury Charms Brooch</t>
   </si>
   <si>
-    <t>Broche</t>
-  </si>
-  <si>
     <t>Luxury Gems Necklace</t>
   </si>
   <si>
@@ -254,6 +251,9 @@
   </si>
   <si>
     <t>,</t>
+  </si>
+  <si>
+    <t>brazalete</t>
   </si>
 </sst>
 </file>
@@ -623,8 +623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30D6B608-1422-4B7D-AB23-4CA37C634D12}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -735,241 +735,241 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6">
+    <row r="6" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>10234</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7">
+    <row r="7" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <v>69780</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8">
+    <row r="8" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="2">
         <v>34125</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9">
+    <row r="9" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="2">
         <v>90876</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10">
+    <row r="10" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="2">
         <v>56789</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="2">
+        <v>43210</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11">
-        <v>43210</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="C12" s="2">
+        <v>21987</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="2">
+        <v>65432</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="2">
+        <v>78901</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="2">
+        <v>34567</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E15" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12">
-        <v>21987</v>
-      </c>
-      <c r="D12" t="s">
+    <row r="16" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="2">
+        <v>89012</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13">
-        <v>65432</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="E16" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="2">
+        <v>45678</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14">
+      <c r="E17" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14">
-        <v>78901</v>
-      </c>
-      <c r="D14" t="s">
+    </row>
+    <row r="18" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="2">
+        <v>12345</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15">
-        <v>34567</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="E18" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="2">
         <v>18</v>
       </c>
-      <c r="E15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16">
-        <v>89012</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="B19" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="2">
+        <v>67890</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17">
-        <v>45678</v>
-      </c>
-      <c r="D17" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18">
-        <v>12345</v>
-      </c>
-      <c r="D18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19">
-        <v>67890</v>
-      </c>
-      <c r="D19" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="E19" s="2" t="s">
         <v>21</v>
       </c>
     </row>
@@ -978,7 +978,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C20">
         <v>78205</v>
@@ -990,10 +990,10 @@
         <v>21</v>
       </c>
       <c r="F20" t="s">
+        <v>35</v>
+      </c>
+      <c r="G20" t="s">
         <v>36</v>
-      </c>
-      <c r="G20" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
@@ -1018,7 +1018,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C22">
         <v>87654</v>
@@ -1035,7 +1035,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C23">
         <v>21098</v>
@@ -1052,7 +1052,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C24">
         <v>98765</v>
@@ -1061,7 +1061,7 @@
         <v>8</v>
       </c>
       <c r="E24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
@@ -1069,7 +1069,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C25">
         <v>34567</v>
@@ -1086,7 +1086,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C26">
         <v>45678</v>
@@ -1103,7 +1103,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C27">
         <v>89012</v>
@@ -1120,7 +1120,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C28">
         <v>12345</v>
@@ -1137,13 +1137,13 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C29">
         <v>67890</v>
       </c>
       <c r="D29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E29" t="s">
         <v>9</v>
@@ -1157,10 +1157,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B80F98F-DB43-4187-8A48-EDD5307C637C}">
-  <dimension ref="B2:D17"/>
+  <dimension ref="B2:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:D9"/>
+      <selection activeCell="B12" sqref="B12:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1172,170 +1172,174 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C2" s="1">
-        <v>54</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C3" s="1">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C4" s="1">
-        <v>3</v>
+        <v>75</v>
       </c>
       <c r="D4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C5" s="1">
-        <v>41</v>
+        <v>86</v>
       </c>
       <c r="D5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C6" s="1">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B7" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C7" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B8" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C8" s="1">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B9" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C9" s="1">
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B10" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C10" s="1">
-        <v>65</v>
+        <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B11" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C11" s="1">
-        <v>18</v>
+        <v>92</v>
       </c>
       <c r="D11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B12" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C12" s="1">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="D12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B13" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C13" s="1">
-        <v>55</v>
+        <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B14" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C14" s="1">
         <v>82</v>
       </c>
+      <c r="D14" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B15" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C15" s="1">
-        <v>82</v>
+        <v>3</v>
       </c>
       <c r="D15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B16" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" s="1">
+        <v>4</v>
+      </c>
+      <c r="D16" t="s">
         <v>70</v>
       </c>
-      <c r="C16" s="1">
-        <v>8</v>
-      </c>
-      <c r="D16" t="s">
-        <v>71</v>
-      </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C17" s="1">
-        <v>2</v>
-      </c>
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C18" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1348,7 +1352,7 @@
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1358,55 +1362,56 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Correcciones en todas la paginas, falta el .jason
</commit_message>
<xml_diff>
--- a/ProyectoFinal/Libro1.xlsx
+++ b/ProyectoFinal/Libro1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nessa\OneDrive\Escritorio\MisProyectos\Bootcamp\BootcampMakaia\ProyectoFinal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3f218cd78eefd738/Escritorio/MisProyectos/Bootcamp/BootcampMakaia/ProyectoFinal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89823364-3682-4B50-9A08-0C6D9A1B85B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{89823364-3682-4B50-9A08-0C6D9A1B85B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EDACB8C5-D9DD-4B28-BC5B-9ED4C271C6F5}"/>
   <bookViews>
-    <workbookView xWindow="-250" yWindow="490" windowWidth="10400" windowHeight="10070" xr2:uid="{3761D6BA-73E2-48D3-BD59-D312106DBE04}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{3761D6BA-73E2-48D3-BD59-D312106DBE04}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="81">
   <si>
     <t>nombre</t>
   </si>
@@ -254,13 +254,40 @@
   </si>
   <si>
     <t>brazalete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gargantilla: </t>
+  </si>
+  <si>
+    <t>princesa:</t>
+  </si>
+  <si>
+    <t>matine</t>
+  </si>
+  <si>
+    <t>cuerdalarga:</t>
+  </si>
+  <si>
+    <t>XG</t>
+  </si>
+  <si>
+    <t>AA</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>G</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -271,6 +298,18 @@
     <font>
       <sz val="8"/>
       <color rgb="FF374151"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF0D0D0D"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF0D0D0D"/>
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
@@ -301,12 +340,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -623,7 +668,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30D6B608-1422-4B7D-AB23-4CA37C634D12}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
@@ -1157,10 +1202,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B80F98F-DB43-4187-8A48-EDD5307C637C}">
-  <dimension ref="B2:D18"/>
+  <dimension ref="B2:I18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1168,9 +1213,10 @@
     <col min="2" max="2" width="13.81640625" customWidth="1"/>
     <col min="3" max="3" width="5.08984375" customWidth="1"/>
     <col min="4" max="4" width="2.90625" customWidth="1"/>
+    <col min="7" max="7" width="21.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>55</v>
       </c>
@@ -1180,8 +1226,14 @@
       <c r="D2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="G2" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>56</v>
       </c>
@@ -1191,8 +1243,14 @@
       <c r="D3" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="G3" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
         <v>57</v>
       </c>
@@ -1202,8 +1260,14 @@
       <c r="D4" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="G4" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
         <v>58</v>
       </c>
@@ -1213,8 +1277,14 @@
       <c r="D5" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="G5" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
         <v>59</v>
       </c>
@@ -1224,8 +1294,14 @@
       <c r="D6" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="G6" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B7" s="1" t="s">
         <v>60</v>
       </c>
@@ -1236,7 +1312,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B8" s="1" t="s">
         <v>61</v>
       </c>
@@ -1247,7 +1323,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B9" s="1" t="s">
         <v>62</v>
       </c>
@@ -1258,7 +1334,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B10" s="1" t="s">
         <v>63</v>
       </c>
@@ -1269,7 +1345,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B11" s="1" t="s">
         <v>64</v>
       </c>
@@ -1280,7 +1356,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B12" s="1" t="s">
         <v>65</v>
       </c>
@@ -1291,7 +1367,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B13" s="1" t="s">
         <v>66</v>
       </c>
@@ -1302,7 +1378,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B14" s="1" t="s">
         <v>67</v>
       </c>
@@ -1313,7 +1389,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B15" s="1" t="s">
         <v>68</v>
       </c>
@@ -1324,7 +1400,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B16" s="1" t="s">
         <v>69</v>
       </c>
@@ -1352,7 +1428,7 @@
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection sqref="A1:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>